<commit_message>
Update Námskeið verkfræðideildar vor og haust 2022 með undanförum.xlsx
</commit_message>
<xml_diff>
--- a/Námskeið verkfræðideildar vor og haust 2022 með undanförum.xlsx
+++ b/Námskeið verkfræðideildar vor og haust 2022 með undanförum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karitasetnaelmarsdottir/Documents/GitHub/LIKX2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9601A7D0-14DE-E946-A164-E3D7C819D5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E4BB4D-B114-6041-ABC8-8FCE99508B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2380" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2396" uniqueCount="645">
   <si>
     <t>CourseCode</t>
   </si>
@@ -2435,8 +2435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3874,6 +3874,9 @@
       <c r="D36" t="s">
         <v>15</v>
       </c>
+      <c r="E36" t="s">
+        <v>427</v>
+      </c>
       <c r="F36">
         <v>8</v>
       </c>
@@ -3988,6 +3991,9 @@
       <c r="D39" t="s">
         <v>15</v>
       </c>
+      <c r="E39" t="s">
+        <v>428</v>
+      </c>
       <c r="F39">
         <v>6</v>
       </c>
@@ -4064,6 +4070,9 @@
       <c r="D41" t="s">
         <v>15</v>
       </c>
+      <c r="E41" t="s">
+        <v>427</v>
+      </c>
       <c r="F41">
         <v>8</v>
       </c>
@@ -4143,6 +4152,9 @@
       <c r="D43" t="s">
         <v>15</v>
       </c>
+      <c r="E43" t="s">
+        <v>427</v>
+      </c>
       <c r="F43">
         <v>8</v>
       </c>
@@ -4181,6 +4193,9 @@
       <c r="D44" t="s">
         <v>15</v>
       </c>
+      <c r="E44" t="s">
+        <v>427</v>
+      </c>
       <c r="F44">
         <v>8</v>
       </c>
@@ -4257,6 +4272,9 @@
       <c r="D46" t="s">
         <v>15</v>
       </c>
+      <c r="E46" t="s">
+        <v>427</v>
+      </c>
       <c r="F46">
         <v>8</v>
       </c>
@@ -4333,6 +4351,9 @@
       <c r="D48" t="s">
         <v>15</v>
       </c>
+      <c r="E48" t="s">
+        <v>427</v>
+      </c>
       <c r="F48">
         <v>8</v>
       </c>
@@ -4409,6 +4430,9 @@
       <c r="D50" t="s">
         <v>15</v>
       </c>
+      <c r="E50" t="s">
+        <v>427</v>
+      </c>
       <c r="F50">
         <v>8</v>
       </c>
@@ -4485,6 +4509,9 @@
       <c r="D52" t="s">
         <v>15</v>
       </c>
+      <c r="E52" t="s">
+        <v>427</v>
+      </c>
       <c r="F52">
         <v>8</v>
       </c>
@@ -4523,6 +4550,9 @@
       <c r="D53" t="s">
         <v>15</v>
       </c>
+      <c r="E53" t="s">
+        <v>428</v>
+      </c>
       <c r="F53">
         <v>6</v>
       </c>
@@ -5281,6 +5311,9 @@
       <c r="D72" t="s">
         <v>498</v>
       </c>
+      <c r="E72" t="s">
+        <v>427</v>
+      </c>
       <c r="F72">
         <v>6</v>
       </c>
@@ -5357,6 +5390,9 @@
       <c r="D74" t="s">
         <v>498</v>
       </c>
+      <c r="E74" t="s">
+        <v>427</v>
+      </c>
       <c r="F74">
         <v>6</v>
       </c>
@@ -5559,6 +5595,9 @@
       <c r="D79" t="s">
         <v>498</v>
       </c>
+      <c r="E79" t="s">
+        <v>427</v>
+      </c>
       <c r="F79">
         <v>6</v>
       </c>
@@ -5597,6 +5636,9 @@
       <c r="D80" t="s">
         <v>498</v>
       </c>
+      <c r="E80" t="s">
+        <v>427</v>
+      </c>
       <c r="F80">
         <v>6</v>
       </c>
@@ -5676,6 +5718,9 @@
       <c r="D82" t="s">
         <v>498</v>
       </c>
+      <c r="E82" t="s">
+        <v>427</v>
+      </c>
       <c r="F82">
         <v>6</v>
       </c>
@@ -5792,6 +5837,9 @@
       </c>
       <c r="D85" t="s">
         <v>498</v>
+      </c>
+      <c r="E85" t="s">
+        <v>427</v>
       </c>
       <c r="F85">
         <v>6</v>

</xml_diff>

<commit_message>
Bæta inn semesterType í excel
</commit_message>
<xml_diff>
--- a/Námskeið verkfræðideildar vor og haust 2022 með undanförum.xlsx
+++ b/Námskeið verkfræðideildar vor og haust 2022 með undanförum.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karitasetnaelmarsdottir/Documents/GitHub/LIKX2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aslaugsol/Documents/GitHub/LIKX2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E4BB4D-B114-6041-ABC8-8FCE99508B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9874FF17-E371-A54B-97FA-6FDA61E62652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2860" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Námskeið" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2396" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2439" uniqueCount="646">
   <si>
     <t>CourseCode</t>
   </si>
@@ -2033,6 +2033,9 @@
   </si>
   <si>
     <t>&lt;p&gt;Kennt í 12 vikur. Fyrirlestrar og dæmatímar.  Aukatímar í hagnýtri forritun verða í boði.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>1V??</t>
   </si>
 </sst>
 </file>
@@ -2435,8 +2438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="E112" sqref="E112"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2753,6 +2756,9 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
+      <c r="E8" t="s">
+        <v>427</v>
+      </c>
       <c r="F8">
         <v>6</v>
       </c>
@@ -3119,6 +3125,9 @@
       <c r="D17" t="s">
         <v>15</v>
       </c>
+      <c r="E17" t="s">
+        <v>427</v>
+      </c>
       <c r="F17">
         <v>6</v>
       </c>
@@ -3485,6 +3494,9 @@
       <c r="D26" t="s">
         <v>15</v>
       </c>
+      <c r="E26" t="s">
+        <v>427</v>
+      </c>
       <c r="F26">
         <v>6</v>
       </c>
@@ -3523,6 +3535,9 @@
       <c r="D27" t="s">
         <v>15</v>
       </c>
+      <c r="E27" t="s">
+        <v>427</v>
+      </c>
       <c r="F27">
         <v>6</v>
       </c>
@@ -3643,6 +3658,9 @@
       <c r="D30" t="s">
         <v>15</v>
       </c>
+      <c r="E30" t="s">
+        <v>427</v>
+      </c>
       <c r="F30">
         <v>6</v>
       </c>
@@ -3681,6 +3699,9 @@
       <c r="D31" t="s">
         <v>15</v>
       </c>
+      <c r="E31" t="s">
+        <v>427</v>
+      </c>
       <c r="F31">
         <v>6</v>
       </c>
@@ -3760,6 +3781,9 @@
       <c r="D33" t="s">
         <v>15</v>
       </c>
+      <c r="E33" t="s">
+        <v>427</v>
+      </c>
       <c r="F33">
         <v>6</v>
       </c>
@@ -3798,6 +3822,9 @@
       <c r="D34" t="s">
         <v>15</v>
       </c>
+      <c r="E34" t="s">
+        <v>427</v>
+      </c>
       <c r="F34">
         <v>6</v>
       </c>
@@ -3836,6 +3863,9 @@
       <c r="D35" t="s">
         <v>15</v>
       </c>
+      <c r="E35" t="s">
+        <v>427</v>
+      </c>
       <c r="F35">
         <v>6</v>
       </c>
@@ -3915,6 +3945,9 @@
       <c r="D37" t="s">
         <v>15</v>
       </c>
+      <c r="E37" t="s">
+        <v>427</v>
+      </c>
       <c r="F37">
         <v>6</v>
       </c>
@@ -3953,6 +3986,9 @@
       <c r="D38" t="s">
         <v>15</v>
       </c>
+      <c r="E38" t="s">
+        <v>428</v>
+      </c>
       <c r="F38">
         <v>6</v>
       </c>
@@ -4032,6 +4068,9 @@
       <c r="D40" t="s">
         <v>15</v>
       </c>
+      <c r="E40" t="s">
+        <v>427</v>
+      </c>
       <c r="F40">
         <v>8</v>
       </c>
@@ -4234,6 +4273,9 @@
       <c r="D45" t="s">
         <v>15</v>
       </c>
+      <c r="E45" t="s">
+        <v>427</v>
+      </c>
       <c r="F45">
         <v>8</v>
       </c>
@@ -4313,6 +4355,9 @@
       <c r="D47" t="s">
         <v>15</v>
       </c>
+      <c r="E47" t="s">
+        <v>427</v>
+      </c>
       <c r="F47">
         <v>8</v>
       </c>
@@ -4392,6 +4437,9 @@
       <c r="D49" t="s">
         <v>15</v>
       </c>
+      <c r="E49" t="s">
+        <v>427</v>
+      </c>
       <c r="F49">
         <v>8</v>
       </c>
@@ -4471,6 +4519,9 @@
       <c r="D51" t="s">
         <v>15</v>
       </c>
+      <c r="E51" t="s">
+        <v>427</v>
+      </c>
       <c r="F51">
         <v>8</v>
       </c>
@@ -4591,6 +4642,9 @@
       <c r="D54" t="s">
         <v>15</v>
       </c>
+      <c r="E54" t="s">
+        <v>615</v>
+      </c>
       <c r="F54">
         <v>30</v>
       </c>
@@ -4667,6 +4721,9 @@
       <c r="D56" t="s">
         <v>15</v>
       </c>
+      <c r="E56" t="s">
+        <v>615</v>
+      </c>
       <c r="F56">
         <v>30</v>
       </c>
@@ -4705,6 +4762,9 @@
       <c r="D57" t="s">
         <v>15</v>
       </c>
+      <c r="E57" t="s">
+        <v>615</v>
+      </c>
       <c r="F57">
         <v>60</v>
       </c>
@@ -4743,6 +4803,9 @@
       <c r="D58" t="s">
         <v>15</v>
       </c>
+      <c r="E58" t="s">
+        <v>615</v>
+      </c>
       <c r="F58">
         <v>60</v>
       </c>
@@ -4781,6 +4844,9 @@
       <c r="D59" t="s">
         <v>15</v>
       </c>
+      <c r="E59" t="s">
+        <v>615</v>
+      </c>
       <c r="F59">
         <v>60</v>
       </c>
@@ -5352,6 +5418,9 @@
       <c r="D73" t="s">
         <v>498</v>
       </c>
+      <c r="E73" t="s">
+        <v>427</v>
+      </c>
       <c r="F73">
         <v>6</v>
       </c>
@@ -5759,6 +5828,9 @@
       <c r="D83" t="s">
         <v>498</v>
       </c>
+      <c r="E83" t="s">
+        <v>427</v>
+      </c>
       <c r="F83">
         <v>6</v>
       </c>
@@ -5920,6 +5992,9 @@
       <c r="D87" t="s">
         <v>498</v>
       </c>
+      <c r="E87" t="s">
+        <v>427</v>
+      </c>
       <c r="F87">
         <v>6</v>
       </c>
@@ -5958,6 +6033,9 @@
       <c r="D88" t="s">
         <v>498</v>
       </c>
+      <c r="E88" t="s">
+        <v>427</v>
+      </c>
       <c r="F88">
         <v>6</v>
       </c>
@@ -5996,6 +6074,9 @@
       <c r="D89" t="s">
         <v>498</v>
       </c>
+      <c r="E89" t="s">
+        <v>427</v>
+      </c>
       <c r="F89">
         <v>6</v>
       </c>
@@ -6034,6 +6115,9 @@
       <c r="D90" t="s">
         <v>498</v>
       </c>
+      <c r="E90" t="s">
+        <v>427</v>
+      </c>
       <c r="F90">
         <v>6</v>
       </c>
@@ -6072,6 +6156,9 @@
       <c r="D91" t="s">
         <v>498</v>
       </c>
+      <c r="E91" t="s">
+        <v>427</v>
+      </c>
       <c r="F91">
         <v>6</v>
       </c>
@@ -6110,6 +6197,9 @@
       <c r="D92" t="s">
         <v>498</v>
       </c>
+      <c r="E92" t="s">
+        <v>427</v>
+      </c>
       <c r="F92">
         <v>6</v>
       </c>
@@ -6148,6 +6238,9 @@
       <c r="D93" t="s">
         <v>498</v>
       </c>
+      <c r="E93" t="s">
+        <v>428</v>
+      </c>
       <c r="F93">
         <v>6</v>
       </c>
@@ -6309,6 +6402,9 @@
       <c r="D97" t="s">
         <v>498</v>
       </c>
+      <c r="E97" t="s">
+        <v>645</v>
+      </c>
       <c r="F97">
         <v>3</v>
       </c>
@@ -6347,6 +6443,9 @@
       <c r="D98" t="s">
         <v>498</v>
       </c>
+      <c r="E98" t="s">
+        <v>427</v>
+      </c>
       <c r="F98">
         <v>6</v>
       </c>
@@ -6385,6 +6484,9 @@
       <c r="D99" t="s">
         <v>498</v>
       </c>
+      <c r="E99" t="s">
+        <v>428</v>
+      </c>
       <c r="F99">
         <v>6</v>
       </c>
@@ -6546,6 +6648,9 @@
       <c r="D103" t="s">
         <v>498</v>
       </c>
+      <c r="E103" t="s">
+        <v>427</v>
+      </c>
       <c r="F103">
         <v>6</v>
       </c>
@@ -6584,6 +6689,9 @@
       <c r="D104" t="s">
         <v>498</v>
       </c>
+      <c r="E104" t="s">
+        <v>427</v>
+      </c>
       <c r="F104">
         <v>6</v>
       </c>
@@ -6663,6 +6771,9 @@
       <c r="D106" t="s">
         <v>498</v>
       </c>
+      <c r="E106" t="s">
+        <v>427</v>
+      </c>
       <c r="F106">
         <v>8</v>
       </c>
@@ -6783,6 +6894,9 @@
       <c r="D109" t="s">
         <v>498</v>
       </c>
+      <c r="E109" t="s">
+        <v>427</v>
+      </c>
       <c r="F109">
         <v>8</v>
       </c>
@@ -6821,6 +6935,9 @@
       <c r="D110" t="s">
         <v>498</v>
       </c>
+      <c r="E110" t="s">
+        <v>427</v>
+      </c>
       <c r="F110">
         <v>8</v>
       </c>
@@ -6900,6 +7017,9 @@
       <c r="D112" t="s">
         <v>498</v>
       </c>
+      <c r="E112" t="s">
+        <v>615</v>
+      </c>
       <c r="F112">
         <v>30</v>
       </c>
@@ -6938,6 +7058,9 @@
       <c r="D113" t="s">
         <v>498</v>
       </c>
+      <c r="E113" t="s">
+        <v>615</v>
+      </c>
       <c r="F113">
         <v>30</v>
       </c>
@@ -7014,6 +7137,9 @@
       <c r="D115" t="s">
         <v>498</v>
       </c>
+      <c r="E115" t="s">
+        <v>615</v>
+      </c>
       <c r="F115">
         <v>60</v>
       </c>
@@ -7052,6 +7178,9 @@
       <c r="D116" t="s">
         <v>498</v>
       </c>
+      <c r="E116" t="s">
+        <v>615</v>
+      </c>
       <c r="F116">
         <v>60</v>
       </c>
@@ -7089,6 +7218,9 @@
       </c>
       <c r="D117" t="s">
         <v>498</v>
+      </c>
+      <c r="E117" t="s">
+        <v>615</v>
       </c>
       <c r="F117">
         <v>60</v>

</xml_diff>